<commit_message>
move MoTaForm.txt to TaiLieu
</commit_message>
<xml_diff>
--- a/TaiLieu/KeHoach.xlsx
+++ b/TaiLieu/KeHoach.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\source\repos\TLMHoang\HeThongSoLienLac\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42122BAC-36B7-4321-BE95-BC8ABD3E86CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1041C5-4A13-4A16-9AE3-F0A21E532B06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01A4F39E-6DED-4548-92AD-D1CB785159CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{01A4F39E-6DED-4548-92AD-D1CB785159CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách Nhóm + Tuần" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Công việc</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Thiết kế web</t>
+  </si>
+  <si>
+    <t>Hoàn thiện web</t>
+  </si>
+  <si>
+    <t>Code chức năng</t>
   </si>
 </sst>
 </file>
@@ -146,7 +152,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-101042A]d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-101042A]d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -483,31 +489,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -553,36 +559,36 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AF1DDD-A992-4308-9F4A-2A2C3DACDCC4}">
   <dimension ref="A3:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:N37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -920,37 +926,37 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
     </row>
     <row r="10" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="36" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="N10" s="29"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="N10" s="28"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -963,10 +969,10 @@
       <c r="C12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="13" t="s">
         <v>2</v>
       </c>
@@ -987,10 +993,10 @@
       <c r="C13" s="21">
         <v>1711061066</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="10" t="s">
         <v>8</v>
       </c>
@@ -1011,10 +1017,10 @@
       <c r="C14" s="24">
         <v>1711060251</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="33"/>
       <c r="F14" s="6">
         <v>1</v>
       </c>
@@ -1035,10 +1041,10 @@
       <c r="C15" s="27">
         <v>1711061367</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="6">
         <v>2</v>
       </c>
@@ -1218,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AEF0AC-0CC3-4A96-A8F0-77A5EBF079FC}">
-  <dimension ref="A7:C23"/>
+  <dimension ref="A7:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="A4:F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1231,11 +1237,11 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1249,7 +1255,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="37">
+      <c r="A10" s="35">
         <v>0</v>
       </c>
       <c r="B10" t="s">
@@ -1296,7 +1302,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C15" t="s">
@@ -1375,7 +1381,56 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update KeHoach.xlsx create DeTai.docx
</commit_message>
<xml_diff>
--- a/TaiLieu/KeHoach.xlsx
+++ b/TaiLieu/KeHoach.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\source\repos\TLMHoang\HeThongSoLienLac\TaiLieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1041C5-4A13-4A16-9AE3-F0A21E532B06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{01A4F39E-6DED-4548-92AD-D1CB785159CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách Nhóm + Tuần" sheetId="1" r:id="rId1"/>
     <sheet name="Kế Hoạch" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="48">
   <si>
     <t>Công việc</t>
   </si>
@@ -102,18 +101,12 @@
     <t>Hoàng</t>
   </si>
   <si>
-    <t>Cả team</t>
-  </si>
-  <si>
     <t>Khởi tạo Project App - Windows</t>
   </si>
   <si>
     <t>Khởi tạo Database</t>
   </si>
   <si>
-    <t>Phong + Trường</t>
-  </si>
-  <si>
     <t>Thiết kế giao diện cho App</t>
   </si>
   <si>
@@ -126,12 +119,6 @@
     <t>Tìm hiểu web</t>
   </si>
   <si>
-    <t>Code 1 chức năng của app</t>
-  </si>
-  <si>
-    <t>Cả team (Hoàng)</t>
-  </si>
-  <si>
     <t>Hoàn thiện app</t>
   </si>
   <si>
@@ -145,12 +132,57 @@
   </si>
   <si>
     <t>Code chức năng</t>
+  </si>
+  <si>
+    <t>Phong</t>
+  </si>
+  <si>
+    <t>Trường</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Code chức năng đăng nhập</t>
+  </si>
+  <si>
+    <t>Code chức năng thêm - xóa - sửa - GV - HS</t>
+  </si>
+  <si>
+    <t>Code trang chủ</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về mobile (Android)</t>
+  </si>
+  <si>
+    <t>Tạo project cho app mobile</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện cho App + Liên kết cac form</t>
+  </si>
+  <si>
+    <t>Code chức năng cho App</t>
+  </si>
+  <si>
+    <t>Kiểm thử hệ thống + sửa lỗi hệ thống</t>
+  </si>
+  <si>
+    <t>GHI CHÚ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm chính </t>
+  </si>
+  <si>
+    <t>Làm phụ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-101042A]d\ mmmm\ yyyy;@"/>
   </numFmts>
@@ -207,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -480,11 +512,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,6 +684,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,11 +1010,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AF1DDD-A992-4308-9F4A-2A2C3DACDCC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q30"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1223,38 +1330,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AEF0AC-0CC3-4A96-A8F0-77A5EBF079FC}">
-  <dimension ref="A7:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A7:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:R43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="46.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="35">
         <v>0</v>
       </c>
@@ -1262,180 +1383,449 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="41"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
       <c r="B21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>5</v>
       </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>6</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
         <v>35</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
         <v>31</v>
       </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A7:C7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
update KeHoac.xlsx create KeHoachThucHienDACS.docx create KeHoachThucHienDACS.xlsx
</commit_message>
<xml_diff>
--- a/TaiLieu/KeHoach.xlsx
+++ b/TaiLieu/KeHoach.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách Nhóm + Tuần" sheetId="1" r:id="rId1"/>
-    <sheet name="Kế Hoạch" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Kế Hoạch" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="153">
   <si>
     <t>Công việc</t>
   </si>
@@ -196,15 +196,9 @@
     <t>Đánh giá</t>
   </si>
   <si>
-    <t>Thiết kế database</t>
-  </si>
-  <si>
     <t>Thiết kế giao diện</t>
   </si>
   <si>
-    <t>10/2 - 16/2/2020</t>
-  </si>
-  <si>
     <t>Code module đăng nhập</t>
   </si>
   <si>
@@ -268,9 +262,6 @@
     <t>diem (theo lop)</t>
   </si>
   <si>
-    <t>Code module Học Sinh - TK</t>
-  </si>
-  <si>
     <t>Code module Admin - giáo viên - Lớp</t>
   </si>
   <si>
@@ -329,6 +320,180 @@
   </si>
   <si>
     <t xml:space="preserve"> web</t>
+  </si>
+  <si>
+    <t>17/2 - 23/2/2020</t>
+  </si>
+  <si>
+    <t>Code module Quản lý tài khoản PHHS</t>
+  </si>
+  <si>
+    <t>Code module Học Sinh</t>
+  </si>
+  <si>
+    <t>Code trigger database</t>
+  </si>
+  <si>
+    <t>Thiết kế database (Table + procduct)</t>
+  </si>
+  <si>
+    <t>24/2 - 1/3/2020</t>
+  </si>
+  <si>
+    <t>2/3 - 9/3/2020</t>
+  </si>
+  <si>
+    <t>2/3 - 8/3/2020</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về web</t>
+  </si>
+  <si>
+    <t>9/3 - 15/3/2020</t>
+  </si>
+  <si>
+    <t>Kiểm thử phần mềm + Fix lỗi</t>
+  </si>
+  <si>
+    <t>Thiết kế trang chủ</t>
+  </si>
+  <si>
+    <t>Thiết kế đăng nhập</t>
+  </si>
+  <si>
+    <t>Thiết kế đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Thiết kế trang thông tin người dùng</t>
+  </si>
+  <si>
+    <t>Thiết kế trang thông tin học sinh</t>
+  </si>
+  <si>
+    <t>Thiết kế trang chuyên cần + Lỗi vi phạm</t>
+  </si>
+  <si>
+    <t>Thiết kế trang điểm + hạnh kiểm</t>
+  </si>
+  <si>
+    <t>Thiết kế trang thông tin giáo viên</t>
+  </si>
+  <si>
+    <t>Trước</t>
+  </si>
+  <si>
+    <t>Sau</t>
+  </si>
+  <si>
+    <t>16/3 - 27/3/2020</t>
+  </si>
+  <si>
+    <t>27/3 - 5/4/2020</t>
+  </si>
+  <si>
+    <t>Code module Trang chủ</t>
+  </si>
+  <si>
+    <t>Code modulde Xem + Sửa thông tin người dùng</t>
+  </si>
+  <si>
+    <t>Code modulde Xem thông tin Giáo viên</t>
+  </si>
+  <si>
+    <t>6/4 - 12/4/2020</t>
+  </si>
+  <si>
+    <t>Code module đăng nhập + Đổi mật khẩu + thông báo nghỉ (nếu có)</t>
+  </si>
+  <si>
+    <t>Code Module Xem điểm</t>
+  </si>
+  <si>
+    <t>Code Module Xem thời khóa biểu + lịch thi</t>
+  </si>
+  <si>
+    <t>Thiết kế trang thời khóa biểu + lịch thi</t>
+  </si>
+  <si>
+    <t>Code Module Xem xem ngày nghỉ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code Module dăng ký nghỉ học có phép </t>
+  </si>
+  <si>
+    <t>Kiểm thử WEB + Fix lỗi</t>
+  </si>
+  <si>
+    <t>Tìm hiểu về Mobile (Android)</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện chính</t>
+  </si>
+  <si>
+    <t>13/4 - 19/4/2020</t>
+  </si>
+  <si>
+    <t>20/4 - 26/4/2020</t>
+  </si>
+  <si>
+    <t>27/4 - 8/5/2020</t>
+  </si>
+  <si>
+    <t>9/5 - 17/5/2020</t>
+  </si>
+  <si>
+    <t>18/5 - 24/5/2020</t>
+  </si>
+  <si>
+    <t>25/5 - 30/502020</t>
+  </si>
+  <si>
+    <t>Kiểm thử APK + Fix lỗi</t>
   </si>
 </sst>
 </file>
@@ -338,7 +503,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-101042A]d\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,16 +555,29 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -760,11 +938,302 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -780,7 +1249,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -871,21 +1339,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -894,8 +1347,91 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1208,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Q30"/>
+  <dimension ref="A3:Q97"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B15"/>
+    <sheetView tabSelected="1" topLeftCell="G76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q96" sqref="Q96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1222,111 +1758,113 @@
     <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="17.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.375" customWidth="1"/>
-    <col min="11" max="11" width="46.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.75" customWidth="1"/>
     <col min="12" max="12" width="19.375" customWidth="1"/>
-    <col min="13" max="13" width="13.875" customWidth="1"/>
+    <col min="13" max="13" width="42.125" customWidth="1"/>
+    <col min="14" max="14" width="18.125" customWidth="1"/>
     <col min="16" max="16" width="20.625" customWidth="1"/>
     <col min="17" max="17" width="17.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="10" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="34" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="N10" s="28"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="N10" s="27"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="32"/>
+      <c r="F12" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>1</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>1711061066</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="10" t="s">
+      <c r="E13" s="32"/>
+      <c r="F13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="10">
         <v>43869</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <v>43870</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
+      <c r="A14" s="21">
         <v>2</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="24">
+      <c r="C14" s="23">
         <v>1711060251</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="6">
-        <v>1</v>
+      <c r="E14" s="32"/>
+      <c r="F14" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="G14" s="4">
         <v>43871</v>
@@ -1336,109 +1874,109 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25">
+      <c r="A15" s="24">
         <v>3</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="26">
         <v>1711061367</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="6">
-        <v>2</v>
-      </c>
-      <c r="G15" s="4">
+      <c r="E15" s="32"/>
+      <c r="F15" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="52">
         <v>43878</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="53">
         <v>43884</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="F16" s="6">
-        <v>3</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="F16" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="52">
         <v>43885</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="53">
         <v>43891</v>
       </c>
     </row>
     <row r="17" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F17" s="6">
-        <v>4</v>
-      </c>
-      <c r="G17" s="4">
+      <c r="F17" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="52">
         <v>43892</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="53">
         <v>43898</v>
       </c>
     </row>
     <row r="18" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F18" s="6">
-        <v>5</v>
-      </c>
-      <c r="G18" s="4">
+      <c r="F18" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="52">
         <v>43899</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="53">
         <v>43905</v>
       </c>
     </row>
     <row r="19" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F19" s="6">
-        <v>6</v>
-      </c>
-      <c r="G19" s="4">
+      <c r="F19" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="52">
         <v>43906</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="53">
         <v>43912</v>
       </c>
     </row>
     <row r="20" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F20" s="6">
-        <v>7</v>
-      </c>
-      <c r="G20" s="4">
+      <c r="F20" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="52">
         <v>43913</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="53">
         <v>43919</v>
       </c>
     </row>
     <row r="21" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F21" s="6">
-        <v>8</v>
-      </c>
-      <c r="G21" s="4">
+      <c r="F21" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="52">
         <v>43920</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="53">
         <v>43926</v>
       </c>
     </row>
     <row r="22" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F22" s="6">
-        <v>9</v>
-      </c>
-      <c r="G22" s="4">
+      <c r="F22" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="52">
         <v>43927</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="53">
         <v>43933</v>
       </c>
     </row>
     <row r="23" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F23" s="6">
-        <v>10</v>
+      <c r="F23" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="G23" s="4">
         <v>43934</v>
@@ -1450,8 +1988,8 @@
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F24" s="6">
-        <v>11</v>
+      <c r="F24" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="G24" s="4">
         <v>43941</v>
@@ -1461,8 +1999,8 @@
       </c>
     </row>
     <row r="25" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F25" s="6">
-        <v>12</v>
+      <c r="F25" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="G25" s="4">
         <v>43948</v>
@@ -1472,8 +2010,8 @@
       </c>
     </row>
     <row r="26" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F26" s="6">
-        <v>13</v>
+      <c r="F26" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="G26" s="4">
         <v>43955</v>
@@ -1483,8 +2021,8 @@
       </c>
     </row>
     <row r="27" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F27" s="6">
-        <v>14</v>
+      <c r="F27" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="G27" s="4">
         <v>43962</v>
@@ -1494,8 +2032,8 @@
       </c>
     </row>
     <row r="28" spans="6:17" x14ac:dyDescent="0.2">
-      <c r="F28" s="6">
-        <v>15</v>
+      <c r="F28" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="G28" s="4">
         <v>43969</v>
@@ -1505,21 +2043,811 @@
       </c>
     </row>
     <row r="29" spans="6:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="7">
-        <v>16</v>
-      </c>
-      <c r="G29" s="8">
+      <c r="F29" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" s="7">
         <v>43976</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="8">
         <v>43981</v>
       </c>
     </row>
     <row r="30" spans="6:17" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="9:14" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="71" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="K35" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="L35" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="N35" s="73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I36" s="54">
+        <v>1</v>
+      </c>
+      <c r="J36" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="K36" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="L36" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="M36" s="55"/>
+      <c r="N36" s="56"/>
+    </row>
+    <row r="37" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I37" s="57"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="L37" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M37" s="58"/>
+      <c r="N37" s="59"/>
+    </row>
+    <row r="38" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I38" s="57"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="L38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M38" s="58"/>
+      <c r="N38" s="59"/>
+    </row>
+    <row r="39" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="75"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="77"/>
+      <c r="L39" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="M39" s="76"/>
+      <c r="N39" s="78"/>
+    </row>
+    <row r="40" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I40" s="79">
+        <v>2</v>
+      </c>
+      <c r="J40" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="K40" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="L40" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M40" s="80"/>
+      <c r="N40" s="81"/>
+    </row>
+    <row r="41" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I41" s="57"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="L41" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M41" s="58"/>
+      <c r="N41" s="59"/>
+    </row>
+    <row r="42" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I42" s="57"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="L42" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M42" s="58"/>
+      <c r="N42" s="59"/>
+    </row>
+    <row r="43" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I43" s="57"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="L43" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M43" s="58"/>
+      <c r="N43" s="59"/>
+    </row>
+    <row r="44" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I44" s="57"/>
+      <c r="J44" s="58"/>
+      <c r="K44" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="L44" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M44" s="58"/>
+      <c r="N44" s="59"/>
+    </row>
+    <row r="45" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="75"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76" t="s">
+        <v>96</v>
+      </c>
+      <c r="L45" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="M45" s="76"/>
+      <c r="N45" s="78"/>
+    </row>
+    <row r="46" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I46" s="67">
+        <v>3</v>
+      </c>
+      <c r="J46" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="K46" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="L46" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="M46" s="68"/>
+      <c r="N46" s="70"/>
+    </row>
+    <row r="47" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I47" s="57"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="L47" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M47" s="58"/>
+      <c r="N47" s="59"/>
+    </row>
+    <row r="48" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I48" s="57"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="L48" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M48" s="58"/>
+      <c r="N48" s="59"/>
+    </row>
+    <row r="49" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I49" s="57"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="60"/>
+      <c r="L49" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M49" s="58"/>
+      <c r="N49" s="59"/>
+    </row>
+    <row r="50" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="82"/>
+      <c r="J50" s="83"/>
+      <c r="K50" s="84"/>
+      <c r="L50" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="M50" s="83"/>
+      <c r="N50" s="86"/>
+    </row>
+    <row r="51" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I51" s="79">
+        <v>4</v>
+      </c>
+      <c r="J51" s="80" t="s">
+        <v>119</v>
+      </c>
+      <c r="K51" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="L51" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M51" s="80"/>
+      <c r="N51" s="81"/>
+    </row>
+    <row r="52" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I52" s="57"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="60"/>
+      <c r="L52" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M52" s="58"/>
+      <c r="N52" s="59"/>
+    </row>
+    <row r="53" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="75"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="77"/>
+      <c r="L53" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="M53" s="76"/>
+      <c r="N53" s="78"/>
+    </row>
+    <row r="54" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I54" s="67">
+        <v>5</v>
+      </c>
+      <c r="J54" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="K54" s="68" t="s">
+        <v>121</v>
+      </c>
+      <c r="L54" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="M54" s="68"/>
+      <c r="N54" s="70"/>
+    </row>
+    <row r="55" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I55" s="57"/>
+      <c r="J55" s="58"/>
+      <c r="K55" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="L55" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M55" s="58"/>
+      <c r="N55" s="59"/>
+    </row>
+    <row r="56" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I56" s="57"/>
+      <c r="J56" s="58"/>
+      <c r="K56" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="L56" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M56" s="58"/>
+      <c r="N56" s="59"/>
+    </row>
+    <row r="57" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I57" s="57"/>
+      <c r="J57" s="58"/>
+      <c r="K57" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="L57" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M57" s="58"/>
+      <c r="N57" s="59"/>
+    </row>
+    <row r="58" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I58" s="57"/>
+      <c r="J58" s="58"/>
+      <c r="K58" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="L58" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M58" s="58"/>
+      <c r="N58" s="59"/>
+    </row>
+    <row r="59" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I59" s="57"/>
+      <c r="J59" s="58"/>
+      <c r="K59" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="L59" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M59" s="58"/>
+      <c r="N59" s="59"/>
+    </row>
+    <row r="60" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I60" s="57"/>
+      <c r="J60" s="58"/>
+      <c r="K60" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="L60" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M60" s="58"/>
+      <c r="N60" s="59"/>
+    </row>
+    <row r="61" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I61" s="57"/>
+      <c r="J61" s="58"/>
+      <c r="K61" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="L61" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M61" s="58"/>
+      <c r="N61" s="59"/>
+    </row>
+    <row r="62" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="82"/>
+      <c r="J62" s="83"/>
+      <c r="K62" s="83" t="s">
+        <v>127</v>
+      </c>
+      <c r="L62" s="85" t="s">
+        <v>15</v>
+      </c>
+      <c r="M62" s="83"/>
+      <c r="N62" s="86"/>
+    </row>
+    <row r="63" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I63" s="79">
+        <v>6</v>
+      </c>
+      <c r="J63" s="80" t="s">
+        <v>132</v>
+      </c>
+      <c r="K63" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="L63" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="M63" s="80"/>
+      <c r="N63" s="81"/>
+    </row>
+    <row r="64" spans="9:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="I64" s="57"/>
+      <c r="J64" s="58"/>
+      <c r="K64" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="L64" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M64" s="58"/>
+      <c r="N64" s="59"/>
+    </row>
+    <row r="65" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I65" s="57"/>
+      <c r="J65" s="58"/>
+      <c r="K65" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="L65" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M65" s="58"/>
+      <c r="N65" s="59"/>
+    </row>
+    <row r="66" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I66" s="75"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="L66" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="M66" s="76"/>
+      <c r="N66" s="78"/>
+    </row>
+    <row r="67" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I67" s="67">
+        <v>7</v>
+      </c>
+      <c r="J67" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="K67" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="L67" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="M67" s="68"/>
+      <c r="N67" s="70"/>
+    </row>
+    <row r="68" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I68" s="57"/>
+      <c r="J68" s="58"/>
+      <c r="K68" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="L68" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M68" s="58"/>
+      <c r="N68" s="59"/>
+    </row>
+    <row r="69" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I69" s="57"/>
+      <c r="J69" s="58"/>
+      <c r="K69" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="L69" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M69" s="58"/>
+      <c r="N69" s="59"/>
+    </row>
+    <row r="70" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I70" s="82"/>
+      <c r="J70" s="83"/>
+      <c r="K70" s="83" t="s">
+        <v>142</v>
+      </c>
+      <c r="L70" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="M70" s="83"/>
+      <c r="N70" s="86"/>
+    </row>
+    <row r="71" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I71" s="79">
+        <v>8</v>
+      </c>
+      <c r="J71" s="80" t="s">
+        <v>146</v>
+      </c>
+      <c r="K71" s="87" t="s">
+        <v>143</v>
+      </c>
+      <c r="L71" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M71" s="80"/>
+      <c r="N71" s="81"/>
+    </row>
+    <row r="72" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I72" s="57"/>
+      <c r="J72" s="58"/>
+      <c r="K72" s="60"/>
+      <c r="L72" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M72" s="58"/>
+      <c r="N72" s="59"/>
+    </row>
+    <row r="73" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I73" s="75"/>
+      <c r="J73" s="76"/>
+      <c r="K73" s="77"/>
+      <c r="L73" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="M73" s="76"/>
+      <c r="N73" s="78"/>
+    </row>
+    <row r="74" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I74" s="67">
+        <v>9</v>
+      </c>
+      <c r="J74" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="K74" s="88" t="s">
+        <v>144</v>
+      </c>
+      <c r="L74" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="M74" s="68"/>
+      <c r="N74" s="70"/>
+    </row>
+    <row r="75" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I75" s="57"/>
+      <c r="J75" s="58"/>
+      <c r="K75" s="60"/>
+      <c r="L75" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M75" s="58"/>
+      <c r="N75" s="59"/>
+    </row>
+    <row r="76" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I76" s="82"/>
+      <c r="J76" s="83"/>
+      <c r="K76" s="84"/>
+      <c r="L76" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="M76" s="83"/>
+      <c r="N76" s="86"/>
+    </row>
+    <row r="77" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I77" s="79">
+        <v>10</v>
+      </c>
+      <c r="J77" s="80" t="s">
+        <v>148</v>
+      </c>
+      <c r="K77" s="80" t="s">
+        <v>145</v>
+      </c>
+      <c r="L77" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M77" s="80"/>
+      <c r="N77" s="81"/>
+    </row>
+    <row r="78" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I78" s="57"/>
+      <c r="J78" s="58"/>
+      <c r="K78" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="L78" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M78" s="58"/>
+      <c r="N78" s="59"/>
+    </row>
+    <row r="79" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I79" s="57"/>
+      <c r="J79" s="58"/>
+      <c r="K79" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="L79" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M79" s="58"/>
+      <c r="N79" s="59"/>
+    </row>
+    <row r="80" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I80" s="57"/>
+      <c r="J80" s="58"/>
+      <c r="K80" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="L80" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M80" s="58"/>
+      <c r="N80" s="59"/>
+    </row>
+    <row r="81" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I81" s="57"/>
+      <c r="J81" s="58"/>
+      <c r="K81" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="L81" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M81" s="58"/>
+      <c r="N81" s="59"/>
+    </row>
+    <row r="82" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I82" s="57"/>
+      <c r="J82" s="58"/>
+      <c r="K82" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="L82" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M82" s="58"/>
+      <c r="N82" s="59"/>
+    </row>
+    <row r="83" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I83" s="57"/>
+      <c r="J83" s="58"/>
+      <c r="K83" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="L83" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M83" s="58"/>
+      <c r="N83" s="59"/>
+    </row>
+    <row r="84" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I84" s="57"/>
+      <c r="J84" s="58"/>
+      <c r="K84" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="L84" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M84" s="58"/>
+      <c r="N84" s="59"/>
+    </row>
+    <row r="85" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="75"/>
+      <c r="J85" s="76"/>
+      <c r="K85" s="76" t="s">
+        <v>127</v>
+      </c>
+      <c r="L85" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="M85" s="76"/>
+      <c r="N85" s="78"/>
+    </row>
+    <row r="86" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I86" s="67">
+        <v>11</v>
+      </c>
+      <c r="J86" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="K86" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="L86" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="M86" s="68"/>
+      <c r="N86" s="70"/>
+    </row>
+    <row r="87" spans="9:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="I87" s="57"/>
+      <c r="J87" s="58"/>
+      <c r="K87" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="L87" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M87" s="58"/>
+      <c r="N87" s="59"/>
+    </row>
+    <row r="88" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I88" s="57"/>
+      <c r="J88" s="58"/>
+      <c r="K88" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="L88" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="M88" s="58"/>
+      <c r="N88" s="59"/>
+    </row>
+    <row r="89" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I89" s="82"/>
+      <c r="J89" s="83"/>
+      <c r="K89" s="83" t="s">
+        <v>135</v>
+      </c>
+      <c r="L89" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="M89" s="83"/>
+      <c r="N89" s="86"/>
+    </row>
+    <row r="90" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I90" s="79">
+        <v>12</v>
+      </c>
+      <c r="J90" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="K90" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="L90" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="M90" s="80"/>
+      <c r="N90" s="81"/>
+    </row>
+    <row r="91" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I91" s="57"/>
+      <c r="J91" s="58"/>
+      <c r="K91" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="L91" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M91" s="58"/>
+      <c r="N91" s="59"/>
+    </row>
+    <row r="92" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I92" s="57"/>
+      <c r="J92" s="58"/>
+      <c r="K92" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="L92" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M92" s="58"/>
+      <c r="N92" s="59"/>
+    </row>
+    <row r="93" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I93" s="75"/>
+      <c r="J93" s="76"/>
+      <c r="K93" s="76" t="s">
+        <v>142</v>
+      </c>
+      <c r="L93" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="M93" s="76"/>
+      <c r="N93" s="78"/>
+    </row>
+    <row r="94" spans="9:14" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="I94" s="67">
+        <v>13</v>
+      </c>
+      <c r="J94" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="K94" s="88" t="s">
+        <v>152</v>
+      </c>
+      <c r="L94" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="M94" s="68"/>
+      <c r="N94" s="70"/>
+    </row>
+    <row r="95" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I95" s="57"/>
+      <c r="J95" s="58"/>
+      <c r="K95" s="60"/>
+      <c r="L95" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M95" s="58"/>
+      <c r="N95" s="59"/>
+    </row>
+    <row r="96" spans="9:14" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I96" s="62"/>
+      <c r="J96" s="63"/>
+      <c r="K96" s="64"/>
+      <c r="L96" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="M96" s="63"/>
+      <c r="N96" s="66"/>
+    </row>
+    <row r="97" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="K74:K76"/>
+    <mergeCell ref="K94:K96"/>
+    <mergeCell ref="K51:K53"/>
+    <mergeCell ref="K48:K50"/>
+    <mergeCell ref="K71:K73"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A3:N3"/>
+    <mergeCell ref="K38:K39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1528,10 +2856,308 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:P21"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" customWidth="1"/>
+    <col min="14" max="14" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C3" s="15"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C5" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="N5" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="C6" s="15"/>
+      <c r="J6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="O8" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="I9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" t="s">
+        <v>88</v>
+      </c>
+      <c r="O9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="I10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" t="s">
+        <v>91</v>
+      </c>
+      <c r="O10" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="I11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="I12" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" t="s">
+        <v>90</v>
+      </c>
+      <c r="O12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="I13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" t="s">
+        <v>92</v>
+      </c>
+      <c r="O13" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="I14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" t="s">
+        <v>33</v>
+      </c>
+      <c r="P14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+    </row>
+    <row r="17" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="N5:P5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="N4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:S22"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1542,23 +3168,23 @@
     <col min="16" max="16" width="20.125" customWidth="1"/>
     <col min="17" max="17" width="31.625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" customWidth="1"/>
+    <col min="19" max="19" width="25.875" customWidth="1"/>
     <col min="20" max="20" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:20" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1596,7 +3222,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="35">
+      <c r="A10" s="34">
         <v>0</v>
       </c>
       <c r="B10" t="s">
@@ -1615,12 +3241,12 @@
         <v>1</v>
       </c>
       <c r="P10" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q10" t="s">
         <v>55</v>
       </c>
-      <c r="Q10" t="s">
-        <v>57</v>
-      </c>
-      <c r="R10" s="41" t="s">
+      <c r="R10" s="40" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1641,9 +3267,9 @@
         <v>36</v>
       </c>
       <c r="Q11" t="s">
-        <v>54</v>
-      </c>
-      <c r="R11" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="R11" s="40" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1652,7 +3278,7 @@
       <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="R12" s="41" t="s">
+      <c r="R12" s="40" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1665,9 +3291,9 @@
         <v>36</v>
       </c>
       <c r="Q13" t="s">
-        <v>53</v>
-      </c>
-      <c r="R13" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="R13" s="40" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1682,10 +3308,16 @@
       <c r="E14" t="s">
         <v>36</v>
       </c>
+      <c r="Q14" t="s">
+        <v>54</v>
+      </c>
+      <c r="R14" s="40" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>42</v>
       </c>
       <c r="D15" t="s">
@@ -1695,10 +3327,10 @@
         <v>36</v>
       </c>
       <c r="Q15" t="s">
-        <v>78</v>
-      </c>
-      <c r="R15" s="41" t="s">
-        <v>15</v>
+        <v>96</v>
+      </c>
+      <c r="R15" s="40" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -1706,14 +3338,20 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>36</v>
+      <c r="C16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16" t="s">
+        <v>100</v>
       </c>
       <c r="Q16" t="s">
-        <v>77</v>
-      </c>
-      <c r="R16" s="41" t="s">
-        <v>17</v>
+        <v>98</v>
+      </c>
+      <c r="R16" s="40" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -1724,9 +3362,9 @@
         <v>36</v>
       </c>
       <c r="Q17" t="s">
-        <v>59</v>
-      </c>
-      <c r="R17" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="R17" s="40" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1741,10 +3379,10 @@
         <v>36</v>
       </c>
       <c r="Q18" t="s">
-        <v>56</v>
-      </c>
-      <c r="R18" s="41" t="s">
-        <v>15</v>
+        <v>97</v>
+      </c>
+      <c r="R18" s="40" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.2">
@@ -1758,14 +3396,14 @@
       <c r="E19" t="s">
         <v>36</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="I19" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="46"/>
+      <c r="J19" s="49"/>
       <c r="Q19" t="s">
-        <v>58</v>
-      </c>
-      <c r="R19" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="R19" s="40" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1783,11 +3421,17 @@
       <c r="E20" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="38" t="s">
+      <c r="I20" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="37" t="s">
         <v>46</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>75</v>
+      </c>
+      <c r="R20" s="40" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1806,16 +3450,16 @@
       <c r="E21" t="s">
         <v>36</v>
       </c>
-      <c r="I21" s="39" t="s">
+      <c r="I21" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="40" t="s">
+      <c r="J21" s="39" t="s">
         <v>47</v>
       </c>
       <c r="Q21" t="s">
-        <v>60</v>
-      </c>
-      <c r="R21" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="R21" s="40" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1824,6 +3468,12 @@
       <c r="B22" t="s">
         <v>29</v>
       </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
@@ -1855,7 +3505,7 @@
       <c r="B25" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1888,7 +3538,7 @@
       <c r="B28" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D28" t="s">
@@ -1914,7 +3564,7 @@
       <c r="E29" t="s">
         <v>35</v>
       </c>
-      <c r="I29" s="20" t="s">
+      <c r="I29" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1934,7 +3584,7 @@
       <c r="E30" t="s">
         <v>35</v>
       </c>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1954,7 +3604,7 @@
       <c r="E31" t="s">
         <v>35</v>
       </c>
-      <c r="I31" s="26" t="s">
+      <c r="I31" s="25" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2119,219 +3769,6 @@
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="I19:J19"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:K21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C1" s="16"/>
-    </row>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C2" s="16"/>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C3" s="16"/>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C4" s="16"/>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C5" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="J5" t="s">
-        <v>97</v>
-      </c>
-      <c r="K5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C6" s="16"/>
-    </row>
-    <row r="7" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="16"/>
-    </row>
-    <row r="8" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="50" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="I9" t="s">
-        <v>91</v>
-      </c>
-      <c r="J9" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="I10" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="I11" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="I12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="I13" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="I14" t="s">
-        <v>96</v>
-      </c>
-      <c r="J14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-    </row>
-    <row r="16" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-    </row>
-    <row r="17" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="16"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="16"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="16"/>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -2352,82 +3789,82 @@
   <sheetData>
     <row r="13" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>